<commit_message>
added a Capstone requirements spreadsheet, to track all the requirments
</commit_message>
<xml_diff>
--- a/data_files/Per Scholas Capstone Requirements.xlsx
+++ b/data_files/Per Scholas Capstone Requirements.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="77">
   <si>
     <t>Req-1.1</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Transaction Details Module</t>
+  </si>
+  <si>
+    <t>Testing inputs</t>
   </si>
   <si>
     <t xml:space="preserve">Used to display the transactions made by customers living in a given zip code for a given month and year. Order by day in descending order.
@@ -258,7 +261,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -312,6 +315,11 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -439,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -515,6 +523,12 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -530,13 +544,13 @@
     <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -987,7 +1001,9 @@
         <v>28</v>
       </c>
       <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
+      <c r="D17" s="27" t="s">
+        <v>29</v>
+      </c>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
@@ -1016,10 +1032,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19">
@@ -1027,10 +1043,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20">
@@ -1038,21 +1054,23 @@
         <v>0</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
+      <c r="D21" s="28" t="s">
+        <v>29</v>
+      </c>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
       <c r="G21" s="25"/>
@@ -1081,9 +1099,9 @@
         <v>0</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="27">
+        <v>38</v>
+      </c>
+      <c r="D22" s="29">
         <v>1.23455652E8</v>
       </c>
     </row>
@@ -1092,9 +1110,9 @@
         <v>0</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="27">
+        <v>39</v>
+      </c>
+      <c r="D23" s="29">
         <v>1.23455652E8</v>
       </c>
     </row>
@@ -1103,10 +1121,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25">
@@ -1114,53 +1132,53 @@
         <v>0</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="1"/>
     </row>
     <row r="27">
-      <c r="A27" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="28" t="s">
+      <c r="A27" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="28"/>
-      <c r="P27" s="28"/>
-      <c r="Q27" s="28"/>
-      <c r="R27" s="28"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="28"/>
-      <c r="U27" s="28"/>
-      <c r="V27" s="28"/>
-      <c r="W27" s="28"/>
-      <c r="X27" s="28"/>
-      <c r="Y27" s="28"/>
-      <c r="Z27" s="28"/>
+      <c r="B27" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+      <c r="W27" s="30"/>
+      <c r="X27" s="30"/>
+      <c r="Y27" s="30"/>
+      <c r="Z27" s="30"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="b">
         <v>0</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29">
@@ -1168,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30">
@@ -1176,50 +1194,50 @@
         <v>0</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" s="1"/>
     </row>
     <row r="32">
-      <c r="A32" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="29" t="s">
+      <c r="A32" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
-      <c r="O32" s="29"/>
-      <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
-      <c r="R32" s="29"/>
-      <c r="S32" s="29"/>
-      <c r="T32" s="29"/>
-      <c r="U32" s="29"/>
-      <c r="V32" s="29"/>
-      <c r="W32" s="29"/>
-      <c r="X32" s="29"/>
-      <c r="Y32" s="29"/>
-      <c r="Z32" s="29"/>
+      <c r="B32" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="31"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="31"/>
+      <c r="V32" s="31"/>
+      <c r="W32" s="31"/>
+      <c r="X32" s="31"/>
+      <c r="Y32" s="31"/>
+      <c r="Z32" s="31"/>
     </row>
     <row r="33">
       <c r="A33" s="5" t="b">
         <v>0</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34">
@@ -1227,7 +1245,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
@@ -1235,50 +1253,50 @@
         <v>0</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="1"/>
     </row>
     <row r="37">
-      <c r="A37" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="30"/>
-      <c r="N37" s="30"/>
-      <c r="O37" s="30"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="30"/>
-      <c r="R37" s="30"/>
-      <c r="S37" s="30"/>
-      <c r="T37" s="30"/>
-      <c r="U37" s="30"/>
-      <c r="V37" s="30"/>
-      <c r="W37" s="30"/>
-      <c r="X37" s="30"/>
-      <c r="Y37" s="30"/>
-      <c r="Z37" s="30"/>
+      <c r="A37" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="32"/>
+      <c r="L37" s="32"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="32"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
+      <c r="W37" s="32"/>
+      <c r="X37" s="32"/>
+      <c r="Y37" s="32"/>
+      <c r="Z37" s="32"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="b">
         <v>0</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39">
@@ -1286,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40">
@@ -1294,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41">
@@ -1302,158 +1320,158 @@
         <v>0</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="1"/>
     </row>
     <row r="43">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
-      <c r="N43" s="31"/>
-      <c r="O43" s="31"/>
-      <c r="P43" s="31"/>
-      <c r="Q43" s="31"/>
-      <c r="R43" s="31"/>
-      <c r="S43" s="31"/>
-      <c r="T43" s="31"/>
-      <c r="U43" s="31"/>
-      <c r="V43" s="31"/>
-      <c r="W43" s="31"/>
-      <c r="X43" s="31"/>
-      <c r="Y43" s="31"/>
-      <c r="Z43" s="31"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="33"/>
+      <c r="Q43" s="33"/>
+      <c r="R43" s="33"/>
+      <c r="S43" s="33"/>
+      <c r="T43" s="33"/>
+      <c r="U43" s="33"/>
+      <c r="V43" s="33"/>
+      <c r="W43" s="33"/>
+      <c r="X43" s="33"/>
+      <c r="Y43" s="33"/>
+      <c r="Z43" s="33"/>
     </row>
     <row r="44">
       <c r="A44" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B44" s="32" t="s">
-        <v>59</v>
+      <c r="B44" s="34" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B45" s="32" t="s">
-        <v>60</v>
+      <c r="B45" s="34" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B46" s="32" t="s">
-        <v>61</v>
+      <c r="B46" s="34" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B47" s="32" t="s">
-        <v>62</v>
+      <c r="B47" s="34" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B48" s="32" t="s">
-        <v>63</v>
+      <c r="B48" s="34" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B49" s="32" t="s">
-        <v>64</v>
+      <c r="B49" s="34" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B50" s="32" t="s">
-        <v>65</v>
+      <c r="B50" s="34" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B51" s="32" t="s">
-        <v>66</v>
+      <c r="B51" s="34" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B52" s="32" t="s">
-        <v>67</v>
+      <c r="B52" s="34" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" s="1"/>
     </row>
     <row r="54">
-      <c r="B54" s="33" t="s">
-        <v>68</v>
+      <c r="B54" s="35" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" s="22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" s="22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" s="22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" s="1"/>
     </row>
     <row r="59">
-      <c r="B59" s="34" t="s">
-        <v>72</v>
+      <c r="B59" s="36" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" s="22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" s="22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63">
@@ -4518,10 +4536,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19">
@@ -4529,10 +4547,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20">
@@ -4540,18 +4558,18 @@
         <v>1</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
@@ -4583,9 +4601,9 @@
         <v>1</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="27">
+        <v>38</v>
+      </c>
+      <c r="D22" s="29">
         <v>1.23455652E8</v>
       </c>
     </row>
@@ -4594,9 +4612,9 @@
         <v>1</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="27">
+        <v>39</v>
+      </c>
+      <c r="D23" s="29">
         <v>1.23455652E8</v>
       </c>
     </row>
@@ -4605,10 +4623,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25">
@@ -4616,53 +4634,53 @@
         <v>1</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="1"/>
     </row>
     <row r="27">
-      <c r="A27" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="28" t="s">
+      <c r="A27" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="28"/>
-      <c r="P27" s="28"/>
-      <c r="Q27" s="28"/>
-      <c r="R27" s="28"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="28"/>
-      <c r="U27" s="28"/>
-      <c r="V27" s="28"/>
-      <c r="W27" s="28"/>
-      <c r="X27" s="28"/>
-      <c r="Y27" s="28"/>
-      <c r="Z27" s="28"/>
+      <c r="B27" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+      <c r="W27" s="30"/>
+      <c r="X27" s="30"/>
+      <c r="Y27" s="30"/>
+      <c r="Z27" s="30"/>
     </row>
     <row r="28">
       <c r="A28" s="24" t="b">
         <v>1</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29">
@@ -4670,7 +4688,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30">
@@ -4678,50 +4696,50 @@
         <v>1</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" s="1"/>
     </row>
     <row r="32">
-      <c r="A32" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="29" t="s">
+      <c r="A32" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
-      <c r="O32" s="29"/>
-      <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
-      <c r="R32" s="29"/>
-      <c r="S32" s="29"/>
-      <c r="T32" s="29"/>
-      <c r="U32" s="29"/>
-      <c r="V32" s="29"/>
-      <c r="W32" s="29"/>
-      <c r="X32" s="29"/>
-      <c r="Y32" s="29"/>
-      <c r="Z32" s="29"/>
+      <c r="B32" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="31"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="31"/>
+      <c r="V32" s="31"/>
+      <c r="W32" s="31"/>
+      <c r="X32" s="31"/>
+      <c r="Y32" s="31"/>
+      <c r="Z32" s="31"/>
     </row>
     <row r="33">
       <c r="A33" s="24" t="b">
         <v>1</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34">
@@ -4729,7 +4747,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35">
@@ -4737,50 +4755,50 @@
         <v>1</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="1"/>
     </row>
     <row r="37">
-      <c r="A37" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="30"/>
-      <c r="N37" s="30"/>
-      <c r="O37" s="30"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="30"/>
-      <c r="R37" s="30"/>
-      <c r="S37" s="30"/>
-      <c r="T37" s="30"/>
-      <c r="U37" s="30"/>
-      <c r="V37" s="30"/>
-      <c r="W37" s="30"/>
-      <c r="X37" s="30"/>
-      <c r="Y37" s="30"/>
-      <c r="Z37" s="30"/>
+      <c r="A37" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="32"/>
+      <c r="L37" s="32"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="32"/>
+      <c r="Q37" s="32"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+      <c r="U37" s="32"/>
+      <c r="V37" s="32"/>
+      <c r="W37" s="32"/>
+      <c r="X37" s="32"/>
+      <c r="Y37" s="32"/>
+      <c r="Z37" s="32"/>
     </row>
     <row r="38">
       <c r="A38" s="24" t="b">
         <v>1</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39">
@@ -4788,7 +4806,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40">
@@ -4796,7 +4814,7 @@
         <v>1</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41">
@@ -4804,112 +4822,112 @@
         <v>1</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="1"/>
     </row>
     <row r="43">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="31"/>
-      <c r="N43" s="31"/>
-      <c r="O43" s="31"/>
-      <c r="P43" s="31"/>
-      <c r="Q43" s="31"/>
-      <c r="R43" s="31"/>
-      <c r="S43" s="31"/>
-      <c r="T43" s="31"/>
-      <c r="U43" s="31"/>
-      <c r="V43" s="31"/>
-      <c r="W43" s="31"/>
-      <c r="X43" s="31"/>
-      <c r="Y43" s="31"/>
-      <c r="Z43" s="31"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="33"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="33"/>
+      <c r="Q43" s="33"/>
+      <c r="R43" s="33"/>
+      <c r="S43" s="33"/>
+      <c r="T43" s="33"/>
+      <c r="U43" s="33"/>
+      <c r="V43" s="33"/>
+      <c r="W43" s="33"/>
+      <c r="X43" s="33"/>
+      <c r="Y43" s="33"/>
+      <c r="Z43" s="33"/>
     </row>
     <row r="44">
       <c r="A44" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B44" s="32" t="s">
-        <v>59</v>
+      <c r="B44" s="34" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="B45" s="32" t="s">
-        <v>60</v>
+      <c r="B45" s="34" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B46" s="32" t="s">
-        <v>61</v>
+      <c r="B46" s="34" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B47" s="32" t="s">
-        <v>62</v>
+      <c r="B47" s="34" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B48" s="32" t="s">
-        <v>63</v>
+      <c r="B48" s="34" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B49" s="32" t="s">
-        <v>64</v>
+      <c r="B49" s="34" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="B50" s="32" t="s">
-        <v>65</v>
+      <c r="B50" s="34" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="B51" s="32" t="s">
-        <v>66</v>
+      <c r="B51" s="34" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="B52" s="32" t="s">
-        <v>67</v>
+      <c r="B52" s="34" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="53">

</xml_diff>